<commit_message>
Arreglando las cabeceras del documento de excel
</commit_message>
<xml_diff>
--- a/csvReaderJson/assets/postalP.xlsx
+++ b/csvReaderJson/assets/postalP.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">ShipAdd2</t>
   </si>
   <si>
-    <t xml:space="preserve">ShipAdd 3</t>
+    <t xml:space="preserve">ShipAdd3</t>
   </si>
   <si>
     <t xml:space="preserve">ShipCity</t>
@@ -133,7 +133,7 @@
     <t xml:space="preserve">ItemHSCode</t>
   </si>
   <si>
-    <t xml:space="preserve">Item Quantity</t>
+    <t xml:space="preserve">ItemQuantity</t>
   </si>
   <si>
     <t xml:space="preserve">ItemValue</t>
@@ -8528,8 +8528,8 @@
   </sheetPr>
   <dimension ref="A1:AM501"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO10" activeCellId="0" sqref="AO10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>